<commit_message>
Update word and excel files
</commit_message>
<xml_diff>
--- a/HW/HW2/wolfStudio.xlsx
+++ b/HW/HW2/wolfStudio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/yuval_kogan_e_braude_ac_il/Documents/Desktop/מחשוב ענן - תיקיית פרויקט/cloud-computing-project/HW/HW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{FA84F642-08E9-454D-9BA3-7AB2521B5DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{126A5555-F4B1-463A-B151-7CD4C4E467D7}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{FA84F642-08E9-454D-9BA3-7AB2521B5DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D44790FA-CD47-4C82-A79D-A239259F00B2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,6 +343,10 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
@@ -355,10 +359,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -532,13 +532,13 @@
     <tableColumn id="15" xr3:uid="{531D5D97-AB37-4865-8CB3-6AAA33803F48}" name="שאלון SUS [מצאתי כי המערכת מאוד מסורבלת לשימוש]" dataDxfId="10"/>
     <tableColumn id="16" xr3:uid="{028BCAA0-8FC3-422A-B529-949F3927BF28}" name="שאלון SUS [חשתי בטחון רב כאשר השתמשתי במערכת]" dataDxfId="9"/>
     <tableColumn id="17" xr3:uid="{AF41D11B-D6C0-4EAB-B889-620194C87399}" name="שאלון SUS [עלי ללמוד הרבה דברים לפני שאוכל להשתמש במערכת זו.]" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{BA76415C-AFB4-43A6-9B22-6681FEAF8D6D}" name="כיצד הרגשת במהלך ההתנסות במערכת ?" dataDxfId="2">
+    <tableColumn id="18" xr3:uid="{BA76415C-AFB4-43A6-9B22-6681FEAF8D6D}" name="כיצד הרגשת במהלך ההתנסות במערכת ?" dataDxfId="0">
       <calculatedColumnFormula>(
- (B2 - 1) + (5 - C2) +
- (E2 - 1) + (5 - F2) +
- (G2 - 1) + (5 - H2) +
- (I2 - 1) + (5 - J2) +
- (K2 - 1) + (5 - L2)
+ (H2 - 1) + (5 - I2) +
+ (J2 - 1) + (5 - K2) +
+ (L2 - 1) + (5 - M2) +
+ (N2 - 1) + (5 - O2) +
+ (P2 - 1) + (5 - Q2)
 ) * 2.5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="19" xr3:uid="{1222FD4A-9587-4761-9779-501D55E224FD}" name="האם לדעתך המערכת מותאמת לאוכלוסיה אליה היא מכוונת?" dataDxfId="7"/>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P16" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" topLeftCell="P10" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,13 +992,13 @@
       </c>
       <c r="R2" s="3">
         <f t="shared" ref="R2:R30" si="0">(
- (B2 - 1) + (5 - C2) +
- (E2 - 1) + (5 - F2) +
- (G2 - 1) + (5 - H2) +
- (I2 - 1) + (5 - J2) +
- (K2 - 1) + (5 - L2)
+ (H2 - 1) + (5 - I2) +
+ (J2 - 1) + (5 - K2) +
+ (L2 - 1) + (5 - M2) +
+ (N2 - 1) + (5 - O2) +
+ (P2 - 1) + (5 - Q2)
 ) * 2.5</f>
-        <v>47.5</v>
+        <v>97.5</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>23</v>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="R3" s="3">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>23</v>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>23</v>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="R5" s="3">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>50</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>23</v>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="R8" s="3">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>45</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>23</v>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="R9" s="3">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>100</v>
       </c>
       <c r="T9" s="4" t="s">
         <v>33</v>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="R10" s="3">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>23</v>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="R11" s="3">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>100</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>23</v>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="R12" s="3">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>23</v>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="R13" s="3">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>67.5</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>23</v>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="R14" s="3">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>90</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>23</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="R15" s="3">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="T15" s="4" t="s">
         <v>44</v>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="R16" s="3">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="T16" s="4" t="s">
         <v>46</v>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="R17" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="T17" s="4" t="s">
         <v>48</v>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="R18" s="3">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T18" s="4" t="s">
         <v>31</v>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="R19" s="3">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="T19" s="4" t="s">
         <v>50</v>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="R20" s="3">
         <f t="shared" si="0"/>
-        <v>42.5</v>
+        <v>87.5</v>
       </c>
       <c r="T20" s="4" t="s">
         <v>34</v>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="R21" s="3">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>97.5</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>23</v>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="R22" s="3">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="R23" s="3">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="S23" s="3" t="s">
         <v>67</v>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="R24" s="3">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>87.5</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>23</v>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="R25" s="3">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>97.5</v>
       </c>
       <c r="S25" s="3" t="s">
         <v>23</v>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="R26" s="3">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>82.5</v>
       </c>
       <c r="S26" s="3" t="s">
         <v>23</v>
@@ -2624,7 +2624,7 @@
       </c>
       <c r="R27" s="3">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>97.5</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>61</v>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="R28" s="3">
         <f t="shared" si="0"/>
-        <v>42.5</v>
+        <v>67.5</v>
       </c>
       <c r="S28" s="3" t="s">
         <v>23</v>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="R29" s="3">
         <f t="shared" si="0"/>
-        <v>32.5</v>
+        <v>102.5</v>
       </c>
       <c r="S29" s="3" t="s">
         <v>23</v>
@@ -2815,7 +2815,7 @@
       </c>
       <c r="R30" s="3">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>23</v>
@@ -2832,7 +2832,7 @@
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="R32" s="3">
         <f>SUM(Table1[כיצד הרגשת במהלך ההתנסות במערכת ?])/29</f>
-        <v>45.344827586206897</v>
+        <v>80.517241379310349</v>
       </c>
       <c r="S32" s="3" t="s">
         <v>66</v>
@@ -2840,12 +2840,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"כן"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update word file and HW folder structure
</commit_message>
<xml_diff>
--- a/HW/HW2/wolfStudio.xlsx
+++ b/HW/HW2/wolfStudio.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,8 +15,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -98,6 +101,9 @@
     <t>אלמנטים שיש לשפר במערכת</t>
   </si>
   <si>
+    <t>אלמנט שופר?</t>
+  </si>
+  <si>
     <t>הערות נוספות לגבי המערכת?</t>
   </si>
   <si>
@@ -197,6 +203,9 @@
     <t>לבחור גרף לפי אפשרות ספיציפית</t>
   </si>
   <si>
+    <t xml:space="preserve"> כן</t>
+  </si>
+  <si>
     <t>הכל מדהים אחלה  גרף</t>
   </si>
   <si>
@@ -234,19 +243,13 @@
   </si>
   <si>
     <t>ציון SUS סופי:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> כן</t>
-  </si>
-  <si>
-    <t>אלמנט שופר?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,24 +346,6 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -378,6 +363,10 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -433,6 +422,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -440,13 +436,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -475,6 +464,20 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -512,27 +515,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC9EAEDB-18F2-4813-826C-A2B215771F9D}" name="Table1" displayName="Table1" ref="A1:W30" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC9EAEDB-18F2-4813-826C-A2B215771F9D}" name="Table1" displayName="Table1" ref="A1:W30" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowBorderDxfId="23" tableBorderDxfId="24">
   <autoFilter ref="A1:W30" xr:uid="{DC9EAEDB-18F2-4813-826C-A2B215771F9D}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{9D162B35-072E-4514-A436-5A02D8C20874}" name="Code" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{D56286CB-C077-4951-B670-94FB355F932B}" name="ההתנסות במערכת [הזמן &quot;טס&quot; במהלך ההתנסות]" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{0EC650D1-B41C-4760-BE06-C0C857CFD724}" name="ההתנסות במערכת [ביצעתי את ההתנסות בהנאה רבה]" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{1D18362F-9EBC-4A5E-885D-EEDE68554A48}" name=" [ארצה לבצע את ההתנסות גם בזמני הפנוי]" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{36EBF4B9-0E1C-4908-B0E7-000B6F9AFE6D}" name="ההתנסות במערכת [ההתנסות היתה בעלת משמעות ומטרה]" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{BAF0472E-C46F-4FDB-8B2B-350FB5D2DB85}" name="ההתנסות במערכת [ההתנסות היתה מאתגרת עבורי]" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{02035027-CB1D-4C8D-A6F7-CFE1890E2034}" name="ההתנסות במערכת [התמדתי בהתנסות  גם כאשר הדברים לא התקדמו בצורה טובה]" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{413EF107-4E09-4ADD-B5BD-2AA368278B07}" name="שאלון SUS [הייתי רוצה להשתמש במערכת זו לעיתים תכופות.]" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{EFBC7603-A90A-495F-AF0D-D765331D9BC5}" name="שאלון SUS [מצאתי כי המערכת מסובכת ללא סיבה]" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{2FC93AA1-A8DE-48C1-AD4E-14C9DE242A97}" name="שאלון SUS [חשבתי שהמערכת קלה לשימוש]" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{423B3825-65AC-48FB-A079-2D18FF145D81}" name="שאלון SUS [אזדקק לתמיכת איש טכני כדי שאוכל להשתמש במערכת זו]" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{0F458EFB-C269-4D3B-8808-7A6765F47F63}" name="שאלון SUS [מצאתי כי הפונקציות השונות של המערכת היו מתואמות היטב]" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{F7D2B256-D168-478E-B636-1535C22668D6}" name="שאלון SUS [חשבתי כי היה יותר מידי חוסר עקביות במערכת זו]" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{3C4D3E1E-24D9-4AE9-B08C-5C5535FFDAED}" name="שאלון SUS [לדעתי רוב האנשים יהיו מסוגלים ללמוד להשתמש במערכת זו בקלות]" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{531D5D97-AB37-4865-8CB3-6AAA33803F48}" name="שאלון SUS [מצאתי כי המערכת מאוד מסורבלת לשימוש]" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{028BCAA0-8FC3-422A-B529-949F3927BF28}" name="שאלון SUS [חשתי בטחון רב כאשר השתמשתי במערכת]" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{AF41D11B-D6C0-4EAB-B889-620194C87399}" name="שאלון SUS [עלי ללמוד הרבה דברים לפני שאוכל להשתמש במערכת זו.]" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{BA76415C-AFB4-43A6-9B22-6681FEAF8D6D}" name="כיצד הרגשת במהלך ההתנסות במערכת ?" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{9D162B35-072E-4514-A436-5A02D8C20874}" name="Code" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{D56286CB-C077-4951-B670-94FB355F932B}" name="ההתנסות במערכת [הזמן &quot;טס&quot; במהלך ההתנסות]" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{0EC650D1-B41C-4760-BE06-C0C857CFD724}" name="ההתנסות במערכת [ביצעתי את ההתנסות בהנאה רבה]" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{1D18362F-9EBC-4A5E-885D-EEDE68554A48}" name=" [ארצה לבצע את ההתנסות גם בזמני הפנוי]" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{36EBF4B9-0E1C-4908-B0E7-000B6F9AFE6D}" name="ההתנסות במערכת [ההתנסות היתה בעלת משמעות ומטרה]" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{BAF0472E-C46F-4FDB-8B2B-350FB5D2DB85}" name="ההתנסות במערכת [ההתנסות היתה מאתגרת עבורי]" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{02035027-CB1D-4C8D-A6F7-CFE1890E2034}" name="ההתנסות במערכת [התמדתי בהתנסות  גם כאשר הדברים לא התקדמו בצורה טובה]" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{413EF107-4E09-4ADD-B5BD-2AA368278B07}" name="שאלון SUS [הייתי רוצה להשתמש במערכת זו לעיתים תכופות.]" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{EFBC7603-A90A-495F-AF0D-D765331D9BC5}" name="שאלון SUS [מצאתי כי המערכת מסובכת ללא סיבה]" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{2FC93AA1-A8DE-48C1-AD4E-14C9DE242A97}" name="שאלון SUS [חשבתי שהמערכת קלה לשימוש]" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{423B3825-65AC-48FB-A079-2D18FF145D81}" name="שאלון SUS [אזדקק לתמיכת איש טכני כדי שאוכל להשתמש במערכת זו]" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{0F458EFB-C269-4D3B-8808-7A6765F47F63}" name="שאלון SUS [מצאתי כי הפונקציות השונות של המערכת היו מתואמות היטב]" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{F7D2B256-D168-478E-B636-1535C22668D6}" name="שאלון SUS [חשבתי כי היה יותר מידי חוסר עקביות במערכת זו]" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{3C4D3E1E-24D9-4AE9-B08C-5C5535FFDAED}" name="שאלון SUS [לדעתי רוב האנשים יהיו מסוגלים ללמוד להשתמש במערכת זו בקלות]" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{531D5D97-AB37-4865-8CB3-6AAA33803F48}" name="שאלון SUS [מצאתי כי המערכת מאוד מסורבלת לשימוש]" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{028BCAA0-8FC3-422A-B529-949F3927BF28}" name="שאלון SUS [חשתי בטחון רב כאשר השתמשתי במערכת]" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{AF41D11B-D6C0-4EAB-B889-620194C87399}" name="שאלון SUS [עלי ללמוד הרבה דברים לפני שאוכל להשתמש במערכת זו.]" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{BA76415C-AFB4-43A6-9B22-6681FEAF8D6D}" name="כיצד הרגשת במהלך ההתנסות במערכת ?" dataDxfId="5">
       <calculatedColumnFormula>(
  (H2 - 1) + (5 - I2) +
  (J2 - 1) + (5 - K2) +
@@ -541,11 +544,11 @@
  (P2 - 1) + (5 - Q2)
 ) * 2.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{1222FD4A-9587-4761-9779-501D55E224FD}" name="האם לדעתך המערכת מותאמת לאוכלוסיה אליה היא מכוונת?" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{AFFB68BD-34CD-46D6-9E3E-30133C00800F}" name="אלמנטים שאהבתי במערכת" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{19BEC92F-FB81-43B2-8A23-5DB6711D9562}" name="אלמנטים שיש לשפר במערכת" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{3999F82B-6BD0-486B-BBC8-EB82225C1FBB}" name="אלמנט שופר?" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{CF75CCF1-23AD-4A51-9FF8-16097B9430B6}" name="הערות נוספות לגבי המערכת?" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{1222FD4A-9587-4761-9779-501D55E224FD}" name="האם לדעתך המערכת מותאמת לאוכלוסיה אליה היא מכוונת?" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{AFFB68BD-34CD-46D6-9E3E-30133C00800F}" name="אלמנטים שאהבתי במערכת" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{19BEC92F-FB81-43B2-8A23-5DB6711D9562}" name="אלמנטים שיש לשפר במערכת" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{3999F82B-6BD0-486B-BBC8-EB82225C1FBB}" name="אלמנט שופר?" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{CF75CCF1-23AD-4A51-9FF8-16097B9430B6}" name="הערות נוספות לגבי המערכת?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -842,34 +845,33 @@
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="46.88671875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="41.21875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="57.109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="48.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="40.77734375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="36.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="55.44140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="57.109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="48.44140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="57.109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="44.21875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="44.33203125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="54.88671875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="33.21875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="47.21875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="63.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="50.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="40.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="48.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="36.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="55.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="57.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="48.42578125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="57.140625" style="3" customWidth="1"/>
+    <col min="15" max="16" width="44.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="54.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="33.28515625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="47.28515625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="63.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="50.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -934,16 +936,16 @@
         <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3">
         <v>7</v>
@@ -1001,22 +1003,22 @@
         <v>97.5</v>
       </c>
       <c r="S2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B3" s="3">
         <v>7</v>
@@ -1068,10 +1070,10 @@
         <v>50</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U3" s="4"/>
       <c r="V3" s="5" t="b">
@@ -1079,9 +1081,9 @@
       </c>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3">
         <v>7</v>
@@ -1133,10 +1135,10 @@
         <v>50</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U4" s="4"/>
       <c r="V4" s="5" t="b">
@@ -1144,9 +1146,9 @@
       </c>
       <c r="W4" s="4"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
@@ -1198,22 +1200,22 @@
         <v>50</v>
       </c>
       <c r="S5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" s="4"/>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="V5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -1265,10 +1267,10 @@
         <v>50</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U6" s="4"/>
       <c r="V6" s="5" t="b">
@@ -1276,9 +1278,9 @@
       </c>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
@@ -1330,10 +1332,10 @@
         <v>50</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="5" t="b">
@@ -1341,9 +1343,9 @@
       </c>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -1392,10 +1394,10 @@
         <v>45</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="5" t="b">
@@ -1403,9 +1405,9 @@
       </c>
       <c r="W8" s="4"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3">
         <v>6</v>
@@ -1457,7 +1459,7 @@
         <v>100</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U9" s="4"/>
       <c r="V9" s="5" t="b">
@@ -1465,9 +1467,9 @@
       </c>
       <c r="W9" s="4"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3">
         <v>7</v>
@@ -1519,10 +1521,10 @@
         <v>50</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U10" s="4"/>
       <c r="V10" s="5" t="b">
@@ -1530,9 +1532,9 @@
       </c>
       <c r="W10" s="4"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3">
         <v>7</v>
@@ -1584,22 +1586,22 @@
         <v>100</v>
       </c>
       <c r="S11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W11" s="4"/>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="V11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B12" s="3">
         <v>7</v>
@@ -1651,24 +1653,24 @@
         <v>100</v>
       </c>
       <c r="S12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -1720,22 +1722,22 @@
         <v>67.5</v>
       </c>
       <c r="S13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="V13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W13" s="4"/>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="U13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="V13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B14" s="3">
         <v>7</v>
@@ -1787,22 +1789,22 @@
         <v>90</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U14" s="4"/>
       <c r="V14" s="5" t="b">
         <v>0</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="3">
         <v>7</v>
@@ -1854,19 +1856,19 @@
         <v>100</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="V15" s="5" t="b">
         <v>0</v>
       </c>
       <c r="W15" s="4"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
@@ -1918,19 +1920,19 @@
         <v>100</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="V16" s="5" t="b">
         <v>0</v>
       </c>
       <c r="W16" s="4"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3">
         <v>6</v>
@@ -1982,19 +1984,19 @@
         <v>100</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U17" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="W17" s="4"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3">
         <v>7</v>
@@ -2046,7 +2048,7 @@
         <v>50</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="5" t="b">
@@ -2054,9 +2056,9 @@
       </c>
       <c r="W18" s="4"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3">
         <v>7</v>
@@ -2108,19 +2110,19 @@
         <v>100</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U19" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="V19" s="5" t="b">
         <v>0</v>
       </c>
       <c r="W19" s="4"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3">
         <v>3</v>
@@ -2172,7 +2174,7 @@
         <v>87.5</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="5" t="b">
@@ -2180,9 +2182,9 @@
       </c>
       <c r="W20" s="4"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23">
       <c r="A21" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3">
         <v>7</v>
@@ -2234,22 +2236,22 @@
         <v>97.5</v>
       </c>
       <c r="S21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W21" s="4"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="U21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="V21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W21" s="4"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -2307,9 +2309,9 @@
       </c>
       <c r="W22" s="4"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3">
         <v>7</v>
@@ -2361,10 +2363,10 @@
         <v>100</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="5" t="b">
@@ -2372,9 +2374,9 @@
       </c>
       <c r="W23" s="4"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3">
         <v>6</v>
@@ -2426,22 +2428,22 @@
         <v>87.5</v>
       </c>
       <c r="S24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V24" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W24" s="4"/>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="U24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="V24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W24" s="4"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B25" s="3">
         <v>7</v>
@@ -2493,22 +2495,22 @@
         <v>97.5</v>
       </c>
       <c r="S25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V25" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W25" s="4"/>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T25" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="U25" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="V25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W25" s="4"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B26" s="3">
         <v>6</v>
@@ -2560,22 +2562,22 @@
         <v>82.5</v>
       </c>
       <c r="S26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W26" s="4"/>
+    </row>
+    <row r="27" spans="1:23">
+      <c r="A27" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T26" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="U26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="V26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W26" s="4"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B27" s="3">
         <v>7</v>
@@ -2627,7 +2629,7 @@
         <v>97.5</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="U27" s="4"/>
       <c r="V27" s="5" t="b">
@@ -2635,9 +2637,9 @@
       </c>
       <c r="W27" s="4"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23">
       <c r="A28" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3">
         <v>4</v>
@@ -2689,10 +2691,10 @@
         <v>67.5</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="5" t="b">
@@ -2700,9 +2702,9 @@
       </c>
       <c r="W28" s="4"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23">
       <c r="A29" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3">
         <v>7</v>
@@ -2751,22 +2753,22 @@
         <v>102.5</v>
       </c>
       <c r="S29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V29" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W29" s="4"/>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="A30" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="U29" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="V29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W29" s="4"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B30" s="3">
         <v>5</v>
@@ -2818,10 +2820,10 @@
         <v>65</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="U30" s="4"/>
       <c r="V30" s="5" t="b">
@@ -2829,23 +2831,23 @@
       </c>
       <c r="W30" s="4"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23">
       <c r="R32" s="3">
         <f>SUM(Table1[כיצד הרגשת במהלך ההתנסות במערכת ?])/29</f>
         <v>80.517241379310349</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"כן"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>